<commit_message>
Planilha de cenários preenchida
</commit_message>
<xml_diff>
--- a/Avaliação - Documentação de Testes.xlsx
+++ b/Avaliação - Documentação de Testes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emers\PycharmProjects\projeto_orange\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57BACBC-2B37-4A63-A507-6C1C1825A2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB61AD2-0D65-46D0-9653-4F20F48A7D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
   <si>
     <t>Equipe</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>Caso de Teste</t>
-  </si>
-  <si>
-    <t>CT-001 - XXXXX</t>
   </si>
   <si>
     <t>Pré-condições</t>
@@ -58,41 +55,90 @@
     <t>Ambiente</t>
   </si>
   <si>
-    <t>CT-002 - XXXXX</t>
-  </si>
-  <si>
-    <t>CT-003 - XXXXX</t>
-  </si>
-  <si>
-    <t>CT-004 - XXXXX</t>
-  </si>
-  <si>
-    <t>CT-005 - XXXXX</t>
-  </si>
-  <si>
-    <t>CT-006 - XXXXX</t>
-  </si>
-  <si>
-    <t>CT-007 - XXXXX</t>
-  </si>
-  <si>
-    <t>CT-008 - XXXXX</t>
-  </si>
-  <si>
-    <t>CT-009 - XXXXX</t>
-  </si>
-  <si>
     <t>Avner Anjos e Emerson Santiago</t>
   </si>
   <si>
     <t>https://opensource-demo.orangehrmlive.com/web/index.php/auth/login</t>
+  </si>
+  <si>
+    <t>Estar logado no sistema e com a página de PIM aberta.</t>
+  </si>
+  <si>
+    <t>1- Clicar no botão [+ Add] na página de PIM;
+2- Preencher o campo 'First Name' com o valor 'Maria';
+3- Preencher o campo 'Middle Name' com o valor 'José';
+4- Preencher o campo 'Last Name' com o valor 'Silva';
+5- Clicar no botão [Save].</t>
+  </si>
+  <si>
+    <t>Sistema deve salvar a inclusão e adicionar o novo usuário na lista de 'employees'.</t>
+  </si>
+  <si>
+    <t>CT-002 - Testar a busca de um usuário - PIM page</t>
+  </si>
+  <si>
+    <t>CT-001 - Testar inclusão de usuário - PIM page</t>
+  </si>
+  <si>
+    <t>1- Preencher o campo 'Employee Name' com o valor 'Maria';
+2- Clicar no botão [Search];
+3- Validar o resultado da busca.</t>
+  </si>
+  <si>
+    <t>O sistema deve exibir o resultado correto para a busca.</t>
+  </si>
+  <si>
+    <t>CT-003 - Testar filtro 'Employment Status' - PIM page</t>
+  </si>
+  <si>
+    <t>1- Clicar no campo 'Employment Status' para expandir a dropdown list;
+2- Selecionar a opção 'FullTime Contract';
+3- Clicar no botão [Search];
+4- Validar que os resultados foram exibidos corretamente.</t>
+  </si>
+  <si>
+    <t>Sistema deve apenas exibir funcionários com status 'Full-Time Contract'.</t>
+  </si>
+  <si>
+    <t>CT-004 - Testar exclusão de usuário - PIM page</t>
+  </si>
+  <si>
+    <t>1- Preencher o campo 'Employee Name' com o valor 'Maria';
+2- Clicar no botão [Search];
+3- Clicar no botão [Excluir] (ícone da lixeira) na coluna 'Actions';
+4- Clicar no botão [Yes, Delete] na pop-up de confirmação;
+5- Validar que a exclusão foi realizada.</t>
+  </si>
+  <si>
+    <t>CT-005 - Testar ordenação ascendente pelo nome - PIM page</t>
+  </si>
+  <si>
+    <t>1- Clicar no ícone de ordenação no quadro de funcionários;
+2- Selecionar a opção 'Ascending';
+3- Validar que a ordenação da lista está sendo feita pelos nomes e de forma ascendente.</t>
+  </si>
+  <si>
+    <t>Sistema deve ordenar os nomes de forma ascendente.</t>
+  </si>
+  <si>
+    <t>CT-006 - Testar o 'Reset' - PIM page</t>
+  </si>
+  <si>
+    <t>1- Clicar no campo 'Employment Status' para expandir a dropdown list;
+2- Selecionar a opção 'FullTime Contract';
+3- Clicar no botão [Search];
+4- Clicar no botão [Reset];
+5- Validar que o reset foi feito.</t>
+  </si>
+  <si>
+    <t>O sistema deve resetar a busca/filtro aplicado.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -142,6 +188,27 @@
       <color theme="10"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -213,7 +280,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -237,6 +304,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -458,15 +537,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B1003"/>
+  <dimension ref="A1:B961"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="76.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -474,8 +553,8 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>19</v>
+      <c r="B1" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -495,7 +574,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
@@ -506,47 +585,49 @@
       <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>3</v>
+      <c r="B7" s="11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="75" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>6</v>
+      <c r="B10" s="10" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="6"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="6"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="6"/>
     </row>
@@ -562,47 +643,49 @@
       <c r="A16" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>11</v>
+      <c r="B16" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="6"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>6</v>
+      <c r="B18" s="10" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="6" t="s">
         <v>6</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" s="6"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" s="6"/>
     </row>
@@ -618,47 +701,49 @@
       <c r="A25" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>12</v>
+      <c r="B25" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="6"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>6</v>
+      <c r="B27" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="6" t="s">
         <v>6</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B29" s="6"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B30" s="6"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31" s="6"/>
     </row>
@@ -674,47 +759,49 @@
       <c r="A34" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>13</v>
+      <c r="B34" s="11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="75" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="6"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>6</v>
+      <c r="B36" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" s="6"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B39" s="6"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B40" s="6"/>
     </row>
@@ -730,47 +817,49 @@
       <c r="A43" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>14</v>
+      <c r="B43" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="60" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="6"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>6</v>
+      <c r="B45" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B46" s="6" t="s">
         <v>6</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B47" s="6"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B48" s="6"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B49" s="6"/>
     </row>
@@ -786,47 +875,49 @@
       <c r="A52" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>15</v>
+      <c r="B52" s="11" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="75" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B53" s="6"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>6</v>
+      <c r="B54" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B55" s="6" t="s">
         <v>6</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B56" s="6"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B57" s="6"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B58" s="6"/>
     </row>
@@ -838,53 +929,33 @@
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B62" s="6"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B65" s="6"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B66" s="6"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B67" s="6"/>
+    <row r="61" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+    </row>
+    <row r="62" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+    </row>
+    <row r="63" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+    </row>
+    <row r="64" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+    </row>
+    <row r="65" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+    </row>
+    <row r="66" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+    </row>
+    <row r="67" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
     </row>
     <row r="68" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
@@ -894,53 +965,33 @@
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B71" s="6"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B74" s="6"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B75" s="6"/>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B76" s="6"/>
+    <row r="70" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+    </row>
+    <row r="71" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+    </row>
+    <row r="72" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
+    </row>
+    <row r="73" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
+    </row>
+    <row r="74" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
+    </row>
+    <row r="75" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+    </row>
+    <row r="76" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
     </row>
     <row r="77" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
@@ -950,53 +1001,33 @@
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B80" s="6"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B83" s="6"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B84" s="6"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B85" s="6"/>
+    <row r="79" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
+    </row>
+    <row r="80" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
+    </row>
+    <row r="81" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
+    </row>
+    <row r="82" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
+    </row>
+    <row r="83" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
+    </row>
+    <row r="84" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
+    </row>
+    <row r="85" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
     </row>
     <row r="86" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="4"/>
@@ -4501,179 +4532,12 @@
     <row r="961" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A961" s="4"/>
       <c r="B961" s="4"/>
-    </row>
-    <row r="962" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A962" s="4"/>
-      <c r="B962" s="4"/>
-    </row>
-    <row r="963" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A963" s="4"/>
-      <c r="B963" s="4"/>
-    </row>
-    <row r="964" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A964" s="4"/>
-      <c r="B964" s="4"/>
-    </row>
-    <row r="965" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A965" s="4"/>
-      <c r="B965" s="4"/>
-    </row>
-    <row r="966" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A966" s="4"/>
-      <c r="B966" s="4"/>
-    </row>
-    <row r="967" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A967" s="4"/>
-      <c r="B967" s="4"/>
-    </row>
-    <row r="968" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A968" s="4"/>
-      <c r="B968" s="4"/>
-    </row>
-    <row r="969" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A969" s="4"/>
-      <c r="B969" s="4"/>
-    </row>
-    <row r="970" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A970" s="4"/>
-      <c r="B970" s="4"/>
-    </row>
-    <row r="971" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A971" s="4"/>
-      <c r="B971" s="4"/>
-    </row>
-    <row r="972" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A972" s="4"/>
-      <c r="B972" s="4"/>
-    </row>
-    <row r="973" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A973" s="4"/>
-      <c r="B973" s="4"/>
-    </row>
-    <row r="974" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A974" s="4"/>
-      <c r="B974" s="4"/>
-    </row>
-    <row r="975" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A975" s="4"/>
-      <c r="B975" s="4"/>
-    </row>
-    <row r="976" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A976" s="4"/>
-      <c r="B976" s="4"/>
-    </row>
-    <row r="977" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A977" s="4"/>
-      <c r="B977" s="4"/>
-    </row>
-    <row r="978" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A978" s="4"/>
-      <c r="B978" s="4"/>
-    </row>
-    <row r="979" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A979" s="4"/>
-      <c r="B979" s="4"/>
-    </row>
-    <row r="980" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A980" s="4"/>
-      <c r="B980" s="4"/>
-    </row>
-    <row r="981" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A981" s="4"/>
-      <c r="B981" s="4"/>
-    </row>
-    <row r="982" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A982" s="4"/>
-      <c r="B982" s="4"/>
-    </row>
-    <row r="983" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A983" s="4"/>
-      <c r="B983" s="4"/>
-    </row>
-    <row r="984" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A984" s="4"/>
-      <c r="B984" s="4"/>
-    </row>
-    <row r="985" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A985" s="4"/>
-      <c r="B985" s="4"/>
-    </row>
-    <row r="986" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A986" s="4"/>
-      <c r="B986" s="4"/>
-    </row>
-    <row r="987" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A987" s="4"/>
-      <c r="B987" s="4"/>
-    </row>
-    <row r="988" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A988" s="4"/>
-      <c r="B988" s="4"/>
-    </row>
-    <row r="989" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A989" s="4"/>
-      <c r="B989" s="4"/>
-    </row>
-    <row r="990" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A990" s="4"/>
-      <c r="B990" s="4"/>
-    </row>
-    <row r="991" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A991" s="4"/>
-      <c r="B991" s="4"/>
-    </row>
-    <row r="992" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A992" s="4"/>
-      <c r="B992" s="4"/>
-    </row>
-    <row r="993" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A993" s="4"/>
-      <c r="B993" s="4"/>
-    </row>
-    <row r="994" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A994" s="4"/>
-      <c r="B994" s="4"/>
-    </row>
-    <row r="995" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A995" s="4"/>
-      <c r="B995" s="4"/>
-    </row>
-    <row r="996" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A996" s="4"/>
-      <c r="B996" s="4"/>
-    </row>
-    <row r="997" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A997" s="4"/>
-      <c r="B997" s="4"/>
-    </row>
-    <row r="998" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A998" s="4"/>
-      <c r="B998" s="4"/>
-    </row>
-    <row r="999" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A999" s="4"/>
-      <c r="B999" s="4"/>
-    </row>
-    <row r="1000" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1000" s="4"/>
-      <c r="B1000" s="4"/>
-    </row>
-    <row r="1001" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1001" s="4"/>
-      <c r="B1001" s="4"/>
-    </row>
-    <row r="1002" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1002" s="4"/>
-      <c r="B1002" s="4"/>
-    </row>
-    <row r="1003" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1003" s="4"/>
-      <c r="B1003" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{6B722049-3818-4BAD-A97C-3B1867CFE64B}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>